<commit_message>
Added to shopping list
</commit_message>
<xml_diff>
--- a/ClientsLists.xlsx
+++ b/ClientsLists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B48F0BD6-6D9D-4522-AB30-F9685715D56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FD4BFA-FACD-47C4-A0D8-498AB48BC2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="3230" windowWidth="16800" windowHeight="9670" activeTab="2" xr2:uid="{3C7FEE18-45D7-4EFE-9D7B-B8684A21AAB4}"/>
+    <workbookView xWindow="1720" yWindow="2890" windowWidth="16800" windowHeight="9670" xr2:uid="{3C7FEE18-45D7-4EFE-9D7B-B8684A21AAB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Beth S." sheetId="1" r:id="rId1"/>
@@ -38,12 +38,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Item</t>
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fruits </t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Basic Dog Food</t>
+  </si>
+  <si>
+    <t>Cat Litter</t>
+  </si>
+  <si>
+    <t>Premium Cat Food</t>
+  </si>
+  <si>
+    <t>Brush</t>
+  </si>
+  <si>
+    <t>Oatmeal Soap</t>
+  </si>
+  <si>
+    <t>Body Butter</t>
+  </si>
+  <si>
+    <t>Catnip</t>
+  </si>
+  <si>
+    <t>Fruits</t>
   </si>
 </sst>
 </file>
@@ -395,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FBF8B8-A47A-4E38-9FDE-D63C4A4CA4D8}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -414,6 +447,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -421,10 +486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64095A3B-B8D7-40C3-BE20-00D2AC7D7084}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -440,6 +505,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -447,10 +544,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA9D931-F57F-49BF-8440-F33E9E7254C2}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,6 +563,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made a dt to list
</commit_message>
<xml_diff>
--- a/ClientsLists.xlsx
+++ b/ClientsLists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FD4BFA-FACD-47C4-A0D8-498AB48BC2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D151C8-62D4-4AA6-92A5-BFFD11BA1F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="2890" windowWidth="16800" windowHeight="9670" xr2:uid="{3C7FEE18-45D7-4EFE-9D7B-B8684A21AAB4}"/>
+    <workbookView xWindow="2060" yWindow="3230" windowWidth="16800" windowHeight="9670" activeTab="2" xr2:uid="{3C7FEE18-45D7-4EFE-9D7B-B8684A21AAB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Beth S." sheetId="1" r:id="rId1"/>
@@ -38,12 +38,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Item</t>
-  </si>
-  <si>
-    <t>Quantity</t>
   </si>
   <si>
     <t>Pizza</t>
@@ -428,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FBF8B8-A47A-4E38-9FDE-D63C4A4CA4D8}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,44 +436,29 @@
     <col min="1" max="1" width="16.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -486,10 +468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64095A3B-B8D7-40C3-BE20-00D2AC7D7084}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,44 +479,29 @@
     <col min="1" max="1" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>8</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -544,10 +511,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA9D931-F57F-49BF-8440-F33E9E7254C2}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -555,44 +522,29 @@
     <col min="1" max="1" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>